<commit_message>
Added Mom and Dad's address
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="179">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -558,13 +553,16 @@
   </si>
   <si>
     <t>1419 Santanna Dr. Lafeytte, IN 47905</t>
+  </si>
+  <si>
+    <t>1326 River Ave. Harlan, IA 51537</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,7 +648,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="17">
     <dxf>
       <border>
         <left style="thin">
@@ -902,250 +900,6 @@
         <horizontal/>
       </border>
     </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1207,7 +961,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1242,7 +996,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1419,22 +1173,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
@@ -1445,7 +1199,7 @@
     <col min="13" max="13" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="7">
         <v>4</v>
       </c>
@@ -1473,7 +1227,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="6">
         <v>3</v>
       </c>
@@ -1493,7 +1247,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1527,7 +1281,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1568,7 +1322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1577,7 +1331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1620,7 +1374,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1660,7 +1414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1700,7 +1454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1739,8 +1493,11 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1780,7 +1537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1820,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" s="1"/>
       <c r="C12">
         <f t="shared" ref="C12:C62" si="5">IF(D12=4, 1,0)</f>
@@ -1847,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1876,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1916,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1956,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1996,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2036,7 +1793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2077,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2117,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -2157,7 +1914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2197,7 +1954,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -2237,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -2277,7 +2034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -2317,7 +2074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -2357,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2397,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -2437,7 +2194,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -2477,7 +2234,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -2517,7 +2274,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2557,7 +2314,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -2597,7 +2354,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -2637,7 +2394,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -2677,7 +2434,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -2717,7 +2474,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -2757,7 +2514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
@@ -2797,7 +2554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -2837,7 +2594,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13">
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
@@ -2877,7 +2634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
@@ -2917,7 +2674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
@@ -2957,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13">
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
@@ -2997,7 +2754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -3037,7 +2794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13">
       <c r="A43" s="2" t="s">
         <v>52</v>
       </c>
@@ -3077,7 +2834,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13">
       <c r="A44" s="2"/>
       <c r="C44">
         <f t="shared" si="5"/>
@@ -3104,7 +2861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13">
       <c r="B45" s="1"/>
       <c r="C45">
         <f t="shared" si="5"/>
@@ -3131,7 +2888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -3160,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -3204,7 +2961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -3248,7 +3005,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -3292,7 +3049,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -3335,7 +3092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -3378,7 +3135,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -3421,7 +3178,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13">
       <c r="C53">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3447,7 +3204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13">
       <c r="A54" s="1" t="s">
         <v>59</v>
       </c>
@@ -3476,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>58</v>
       </c>
@@ -3516,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -3556,7 +3313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>60</v>
       </c>
@@ -3596,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>126</v>
       </c>
@@ -3636,7 +3393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -3676,7 +3433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -3716,7 +3473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -3756,7 +3513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13">
       <c r="C62">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3782,7 +3539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13">
       <c r="A63" s="1" t="s">
         <v>57</v>
       </c>
@@ -3811,7 +3568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -3851,7 +3608,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -3891,7 +3648,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -3934,7 +3691,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -3974,7 +3731,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -4014,7 +3771,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>71</v>
       </c>
@@ -4054,7 +3811,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>72</v>
       </c>
@@ -4094,7 +3851,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -4135,7 +3892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>80</v>
       </c>
@@ -4176,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -4216,7 +3973,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -4256,7 +4013,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -4296,7 +4053,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -4336,7 +4093,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -4376,7 +4133,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -4417,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>81</v>
       </c>
@@ -4458,7 +4215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>82</v>
       </c>
@@ -4499,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11">
       <c r="A81" t="s">
         <v>85</v>
       </c>
@@ -4539,7 +4296,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11">
       <c r="A82" t="s">
         <v>86</v>
       </c>
@@ -4579,7 +4336,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11">
       <c r="A83" t="s">
         <v>87</v>
       </c>
@@ -4619,7 +4376,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -4660,7 +4417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11">
       <c r="A85" t="s">
         <v>88</v>
       </c>
@@ -4701,7 +4458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11">
       <c r="A86" t="s">
         <v>89</v>
       </c>
@@ -4742,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -4783,7 +4540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11">
       <c r="A88" t="s">
         <v>91</v>
       </c>
@@ -4824,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11">
       <c r="A89" t="s">
         <v>92</v>
       </c>
@@ -4865,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11">
       <c r="A90" t="s">
         <v>93</v>
       </c>
@@ -4906,7 +4663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -4947,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -4988,7 +4745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11">
       <c r="A93" t="s">
         <v>96</v>
       </c>
@@ -5029,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11">
       <c r="A94" t="s">
         <v>97</v>
       </c>
@@ -5070,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11">
       <c r="A95" t="s">
         <v>98</v>
       </c>
@@ -5111,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11">
       <c r="A96" t="s">
         <v>99</v>
       </c>
@@ -5152,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -5193,7 +4950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11">
       <c r="A98" t="s">
         <v>109</v>
       </c>
@@ -5234,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11">
       <c r="A99" t="s">
         <v>110</v>
       </c>
@@ -5275,7 +5032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11">
       <c r="A100" t="s">
         <v>111</v>
       </c>
@@ -5316,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11">
       <c r="A101" t="s">
         <v>112</v>
       </c>
@@ -5357,7 +5114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11">
       <c r="A102" t="s">
         <v>113</v>
       </c>
@@ -5398,7 +5155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11">
       <c r="A103" t="s">
         <v>114</v>
       </c>
@@ -5439,7 +5196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11">
       <c r="C104">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5465,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11">
       <c r="A105" s="1" t="s">
         <v>115</v>
       </c>
@@ -5494,7 +5251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11">
       <c r="A106" s="2" t="s">
         <v>137</v>
       </c>
@@ -5534,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11">
       <c r="A107" t="s">
         <v>116</v>
       </c>
@@ -5574,7 +5331,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11">
       <c r="A108" t="s">
         <v>117</v>
       </c>
@@ -5614,7 +5371,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11">
       <c r="A109" t="s">
         <v>118</v>
       </c>
@@ -5654,7 +5411,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11">
       <c r="A110" t="s">
         <v>119</v>
       </c>
@@ -5694,7 +5451,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11">
       <c r="A111" t="s">
         <v>120</v>
       </c>
@@ -5734,7 +5491,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -5774,7 +5531,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11">
       <c r="A113" t="s">
         <v>122</v>
       </c>
@@ -5814,7 +5571,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -5855,7 +5612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11">
       <c r="A115" t="s">
         <v>124</v>
       </c>
@@ -5896,7 +5653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11">
       <c r="A116" t="s">
         <v>125</v>
       </c>
@@ -5937,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11">
       <c r="A117" t="s">
         <v>127</v>
       </c>
@@ -5977,7 +5734,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11">
       <c r="A118" t="s">
         <v>128</v>
       </c>
@@ -6017,7 +5774,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11">
       <c r="A119" t="s">
         <v>129</v>
       </c>
@@ -6058,7 +5815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11">
       <c r="A120" t="s">
         <v>130</v>
       </c>
@@ -6098,7 +5855,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11">
       <c r="A121" t="s">
         <v>131</v>
       </c>
@@ -6138,7 +5895,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11">
       <c r="A122" t="s">
         <v>132</v>
       </c>
@@ -6179,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11">
       <c r="A123" t="s">
         <v>133</v>
       </c>
@@ -6220,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11">
       <c r="A124" t="s">
         <v>134</v>
       </c>
@@ -6261,7 +6018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11">
       <c r="A125" t="s">
         <v>135</v>
       </c>
@@ -6302,7 +6059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11">
       <c r="A126" t="s">
         <v>136</v>
       </c>
@@ -6343,7 +6100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11">
       <c r="A127" t="s">
         <v>145</v>
       </c>
@@ -6383,7 +6140,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11">
       <c r="A128" t="s">
         <v>146</v>
       </c>
@@ -6411,7 +6168,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11">
       <c r="A129" t="s">
         <v>147</v>
       </c>
@@ -6439,7 +6196,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11">
       <c r="A130" t="s">
         <v>148</v>
       </c>
@@ -6468,7 +6225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11">
       <c r="A131" t="s">
         <v>149</v>
       </c>
@@ -6497,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11">
       <c r="A132" t="s">
         <v>150</v>
       </c>
@@ -6526,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -6555,7 +6312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11">
       <c r="A134" t="s">
         <v>152</v>
       </c>
@@ -6584,7 +6341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11">
       <c r="A135" t="s">
         <v>153</v>
       </c>
@@ -6613,7 +6370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11">
       <c r="A136" t="s">
         <v>157</v>
       </c>
@@ -6653,7 +6410,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11">
       <c r="A137" t="s">
         <v>139</v>
       </c>
@@ -6694,7 +6451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11">
       <c r="A138" t="s">
         <v>140</v>
       </c>
@@ -6735,7 +6492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11">
       <c r="A139" t="s">
         <v>156</v>
       </c>
@@ -6776,7 +6533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11">
       <c r="A140" t="s">
         <v>141</v>
       </c>
@@ -6817,7 +6574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11">
       <c r="A141" t="s">
         <v>158</v>
       </c>
@@ -6858,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -6899,7 +6656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -6940,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -6981,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11">
       <c r="A145" t="s">
         <v>154</v>
       </c>
@@ -7022,7 +6779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11">
       <c r="A146" t="s">
         <v>155</v>
       </c>
@@ -7063,7 +6820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11">
       <c r="A147" t="s">
         <v>83</v>
       </c>
@@ -7104,7 +6861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11">
       <c r="C148">
         <f t="shared" si="21"/>
         <v>0</v>
@@ -7130,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11">
       <c r="A149" s="1" t="s">
         <v>159</v>
       </c>
@@ -7159,7 +6916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11">
       <c r="A150" t="s">
         <v>160</v>
       </c>
@@ -7199,7 +6956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11">
       <c r="A151" t="s">
         <v>161</v>
       </c>
@@ -7239,7 +6996,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11">
       <c r="A152" t="s">
         <v>162</v>
       </c>
@@ -7279,7 +7036,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11">
       <c r="A153" t="s">
         <v>163</v>
       </c>
@@ -7319,7 +7076,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11">
       <c r="A154" t="s">
         <v>164</v>
       </c>
@@ -7359,7 +7116,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11">
       <c r="A155" t="s">
         <v>165</v>
       </c>
@@ -7400,7 +7157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11">
       <c r="A156" t="s">
         <v>166</v>
       </c>
@@ -7441,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11">
       <c r="A157" t="s">
         <v>167</v>
       </c>
@@ -7482,7 +7239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11">
       <c r="A158" t="s">
         <v>168</v>
       </c>
@@ -7523,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11">
       <c r="A159" t="s">
         <v>169</v>
       </c>
@@ -7564,7 +7321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11">
       <c r="A160" t="s">
         <v>170</v>
       </c>
@@ -7604,7 +7361,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11">
       <c r="A161" t="s">
         <v>171</v>
       </c>
@@ -7645,7 +7402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11">
       <c r="A162" t="s">
         <v>172</v>
       </c>
@@ -7686,7 +7443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11">
       <c r="A163" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Updated with Save The Date Info
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="225">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -233,9 +228,6 @@
     <t>Cam Ebner</t>
   </si>
   <si>
-    <t>Ceasar Roca and Anna Po…</t>
-  </si>
-  <si>
     <t>Mi-Sun Bae</t>
   </si>
   <si>
@@ -263,9 +255,6 @@
     <t>Kris and Brent</t>
   </si>
   <si>
-    <t>Brian and Haley</t>
-  </si>
-  <si>
     <t>Ami Yang</t>
   </si>
   <si>
@@ -275,9 +264,6 @@
     <t>Andrea Parker</t>
   </si>
   <si>
-    <t>Katelyn Dv…</t>
-  </si>
-  <si>
     <t>Sam and Tori</t>
   </si>
   <si>
@@ -335,27 +321,15 @@
     <t>Christopher and Kaylea Blount</t>
   </si>
   <si>
-    <t>Drew Stephans and Amanda …</t>
-  </si>
-  <si>
-    <t>Peter and Shannon Happ</t>
-  </si>
-  <si>
     <t>Cory and Katie Brewer</t>
   </si>
   <si>
     <t>Joshua Nation and Mallory Daly</t>
   </si>
   <si>
-    <t>Ginina Vittuci and Guest</t>
-  </si>
-  <si>
     <t xml:space="preserve">Brooke Ulrich </t>
   </si>
   <si>
-    <t>Meg Lees and Fiance</t>
-  </si>
-  <si>
     <t>Christopher Naranjo</t>
   </si>
   <si>
@@ -374,18 +348,9 @@
     <t>Liz and Brent</t>
   </si>
   <si>
-    <t>Melissa and Michael</t>
-  </si>
-  <si>
     <t>Christine &amp; Guest</t>
   </si>
   <si>
-    <t>Dave and Diane Greve</t>
-  </si>
-  <si>
-    <t>Dave and Angela Voge</t>
-  </si>
-  <si>
     <t>Joe and Amy Rueschenberg &amp; Fam</t>
   </si>
   <si>
@@ -467,12 +432,6 @@
     <t>8610 EP True Pkwy, Unit 11005, West Des Moines, IA 50266</t>
   </si>
   <si>
-    <t>11450 Dan Patch Circle, Green Oaks, IL 600448</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check on zip code… lol </t>
-  </si>
-  <si>
     <t>639 N Broadway #538, Los Angeles, CA 90012</t>
   </si>
   <si>
@@ -572,9 +531,6 @@
     <t>Joseph Loescher &amp; Guest</t>
   </si>
   <si>
-    <t>Michael Jerman &amp; Guest</t>
-  </si>
-  <si>
     <t>2394 Quinlan Ave., Dallas Center, IA 50063</t>
   </si>
   <si>
@@ -668,17 +624,83 @@
     <t>1815 Marilyn Lane, Aurora, IL 60505</t>
   </si>
   <si>
-    <t>175 W Julian St. Unit 6, Chicago, IL 60622</t>
-  </si>
-  <si>
     <t>S2881 Willow Ln. Fountain City, WI 54629</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Meg Lees and Zachary Kelch</t>
+  </si>
+  <si>
+    <t>Melissa and Michael Bellinghausen</t>
+  </si>
+  <si>
+    <t>1751 W Julian St. Unit 6, Chicago, IL 60622</t>
+  </si>
+  <si>
+    <t>Peter Happ and Shannon Wilson</t>
+  </si>
+  <si>
+    <t>2323 Fairwind Rd., Apt 107, Houston, TX 77062</t>
+  </si>
+  <si>
+    <t>1919 Huntress Lane, Houston, TX 77062</t>
+  </si>
+  <si>
+    <t>Drew Stephans and Amanda Mueller</t>
+  </si>
+  <si>
+    <t>Michael Jerman &amp; Stacy Solliday</t>
+  </si>
+  <si>
+    <t>Ginina Vittuci and Benjamin Booher</t>
+  </si>
+  <si>
+    <t>Dave and Diane Greve &amp; Fam</t>
+  </si>
+  <si>
+    <t>Dave and Angela Voge &amp; Fam</t>
+  </si>
+  <si>
+    <t>11450 Dan Patch Circle, Green Oaks, IL 60048</t>
+  </si>
+  <si>
+    <t>540 Thomas Ct., Apt 12, Portage, MI 49024</t>
+  </si>
+  <si>
+    <t>200 Water St. Apt 12301, Webser, TX 77598</t>
+  </si>
+  <si>
+    <t>165 Rainbow Dr. #6587 Livingston, TX 7739</t>
+  </si>
+  <si>
+    <t>Brian Killeen</t>
+  </si>
+  <si>
+    <t>Ceasar Roca and Anna Podobas</t>
+  </si>
+  <si>
+    <t>3018 Quill Meadow Drive, League City, TX 77573</t>
+  </si>
+  <si>
+    <t>Katelyn Dvorsky</t>
+  </si>
+  <si>
+    <t>19220 Space Center Blvd, Apt 1335, Houston, TX 77058</t>
+  </si>
+  <si>
+    <t>Included with Logan's other Save-the-Dates</t>
+  </si>
+  <si>
+    <t>Logan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -701,7 +723,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -738,6 +760,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -751,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -763,6 +791,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,22 +1322,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L99" sqref="L99"/>
+      <pane ySplit="4" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O85" sqref="O85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
@@ -1321,80 +1351,80 @@
     <col min="16" max="16" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="7">
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C1">
         <f ca="1">SUMIF(C5:C228,"=1",E6:E228)</f>
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="D1">
         <f>SUM(E5:E139)</f>
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="E1">
         <f>SUMIF(D6:D228,"&gt;1",E6:E228)</f>
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F1">
         <f>SUMIF(D6:D228,"&gt;2",E6:E228)</f>
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="G1">
         <f>SUMIF(D6:D228,"&gt;3",E6:E228)</f>
         <v>130</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="6">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
         <v>91</v>
-      </c>
-      <c r="E2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F2" t="s">
-        <v>93</v>
-      </c>
-      <c r="G2" t="s">
-        <v>94</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C3">
         <f>SUM(K5:K228)</f>
-        <v>123.89999999999989</v>
+        <v>126.09999999999989</v>
       </c>
       <c r="D3">
         <f>SUM(G6:G190)</f>
-        <v>147.80000000000001</v>
+        <v>150.00000000000003</v>
       </c>
       <c r="E3">
         <f>SUM(H:H)</f>
@@ -1418,7 +1448,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1426,7 +1456,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
@@ -1438,19 +1468,19 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" t="s">
         <v>87</v>
       </c>
-      <c r="H4" t="s">
-        <v>88</v>
-      </c>
-      <c r="I4" t="s">
-        <v>89</v>
-      </c>
-      <c r="J4" t="s">
-        <v>90</v>
-      </c>
       <c r="K4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="L4" t="s">
         <v>3</v>
@@ -1462,7 +1492,7 @@
       <c r="O4" s="8"/>
       <c r="P4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1501,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1511,13 +1541,16 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="N6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1557,13 +1590,16 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1603,13 +1639,13 @@
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1649,13 +1685,16 @@
         <v>2</v>
       </c>
       <c r="L9" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="N9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1695,13 +1734,16 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="N10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1743,8 +1785,11 @@
       <c r="N11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="B12" s="1"/>
       <c r="C12">
         <f t="shared" ref="C12:C62" si="5">IF(D12=4, 1,0)</f>
@@ -1771,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1800,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1842,8 +1887,11 @@
       <c r="N14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -1883,13 +1931,16 @@
         <v>1</v>
       </c>
       <c r="L15" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="N15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -1932,7 +1983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -1975,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2017,8 +2068,11 @@
       <c r="N18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2060,8 +2114,11 @@
       <c r="N19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -2104,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2147,7 +2204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
@@ -2189,8 +2246,11 @@
       <c r="N22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
@@ -2230,13 +2290,16 @@
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="N23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
@@ -2279,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -2321,8 +2384,11 @@
       <c r="N25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -2364,8 +2430,11 @@
       <c r="N26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="2" t="s">
         <v>23</v>
       </c>
@@ -2407,8 +2476,11 @@
       <c r="N27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
@@ -2450,8 +2522,11 @@
       <c r="N28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -2493,8 +2568,11 @@
       <c r="N29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
@@ -2536,8 +2614,11 @@
       <c r="N30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -2579,8 +2660,11 @@
       <c r="N31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" s="2" t="s">
         <v>28</v>
       </c>
@@ -2622,8 +2706,11 @@
       <c r="N32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -2665,8 +2752,11 @@
       <c r="N33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -2708,8 +2798,11 @@
       <c r="N34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" s="2" t="s">
         <v>44</v>
       </c>
@@ -2749,13 +2842,16 @@
         <v>2</v>
       </c>
       <c r="L35" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="N35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
         <v>45</v>
       </c>
@@ -2795,13 +2891,16 @@
         <v>2</v>
       </c>
       <c r="L36" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="N36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
@@ -2841,13 +2940,16 @@
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="N37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
@@ -2890,7 +2992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="2" t="s">
         <v>48</v>
       </c>
@@ -2930,13 +3032,16 @@
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="N39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="2" t="s">
         <v>49</v>
       </c>
@@ -2976,16 +3081,16 @@
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>147</v>
-      </c>
-      <c r="M40" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="N40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
         <v>50</v>
       </c>
@@ -3025,13 +3130,16 @@
         <v>1</v>
       </c>
       <c r="L41" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="N41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
         <v>51</v>
       </c>
@@ -3071,15 +3179,15 @@
         <v>2</v>
       </c>
       <c r="M42" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="N42">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B43" s="2">
         <v>2</v>
@@ -3117,13 +3225,16 @@
         <v>0.5</v>
       </c>
       <c r="L43" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="N43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="2"/>
       <c r="C44">
         <f t="shared" si="5"/>
@@ -3150,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="B45" s="1"/>
       <c r="C45">
         <f t="shared" si="5"/>
@@ -3177,7 +3288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="1" t="s">
         <v>31</v>
       </c>
@@ -3209,7 +3320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>32</v>
       </c>
@@ -3256,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -3303,7 +3414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -3350,7 +3461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -3396,7 +3507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -3442,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -3488,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15">
       <c r="C53">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3514,7 +3625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
         <v>58</v>
       </c>
@@ -3543,7 +3654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -3582,14 +3693,16 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L55" t="s">
-        <v>191</v>
-      </c>
-      <c r="N55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L55" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9">
+        <v>1</v>
+      </c>
+      <c r="O55" s="9"/>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -3628,14 +3741,16 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="L56" t="s">
-        <v>163</v>
-      </c>
-      <c r="N56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L56" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9">
+        <v>1</v>
+      </c>
+      <c r="O56" s="9"/>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -3674,16 +3789,18 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L57" t="s">
-        <v>191</v>
-      </c>
-      <c r="N57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L57" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9">
+        <v>1</v>
+      </c>
+      <c r="O57" s="9"/>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -3721,13 +3838,16 @@
         <v>2</v>
       </c>
       <c r="L58" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="N58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -3767,13 +3887,16 @@
         <v>1</v>
       </c>
       <c r="L59" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="N59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -3813,13 +3936,16 @@
         <v>2</v>
       </c>
       <c r="L60" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="N60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -3859,13 +3985,16 @@
         <v>2</v>
       </c>
       <c r="L61" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="N61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="C62">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3891,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="1" t="s">
         <v>56</v>
       </c>
@@ -3920,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -3959,14 +4088,16 @@
         <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
-      <c r="L64" t="s">
-        <v>191</v>
-      </c>
-      <c r="N64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L64" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9">
+        <v>1</v>
+      </c>
+      <c r="O64" s="9"/>
+    </row>
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -4006,13 +4137,16 @@
         <v>1.8</v>
       </c>
       <c r="L65" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="N65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -4051,17 +4185,18 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="L66" t="s">
-        <v>191</v>
-      </c>
-      <c r="M66" t="s">
+      <c r="L66" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M66" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="N66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N66" s="9">
+        <v>1</v>
+      </c>
+      <c r="O66" s="9"/>
+    </row>
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -4100,16 +4235,18 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="L67" t="s">
-        <v>191</v>
-      </c>
-      <c r="N67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L67" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9">
+        <v>1</v>
+      </c>
+      <c r="O67" s="9"/>
+    </row>
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>219</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -4147,15 +4284,18 @@
         <v>1.8</v>
       </c>
       <c r="L68" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="N68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -4166,13 +4306,16 @@
       <c r="F69">
         <v>90</v>
       </c>
-      <c r="N69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9">
+        <v>1</v>
+      </c>
+      <c r="O69" s="9"/>
+    </row>
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -4210,15 +4353,18 @@
         <v>0.9</v>
       </c>
       <c r="L70" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="N70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -4255,16 +4401,18 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="L71" t="s">
-        <v>192</v>
-      </c>
-      <c r="N71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L71" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9">
+        <v>1</v>
+      </c>
+      <c r="O71" s="9"/>
+    </row>
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -4303,9 +4451,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -4343,15 +4491,18 @@
         <v>1.8</v>
       </c>
       <c r="L73" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="N73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>2</v>
@@ -4389,15 +4540,18 @@
         <v>1.8</v>
       </c>
       <c r="L74" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="N74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -4435,15 +4589,18 @@
         <v>1.8</v>
       </c>
       <c r="L75" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="N75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -4481,15 +4638,18 @@
         <v>1.8</v>
       </c>
       <c r="L76" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="N76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -4527,15 +4687,18 @@
         <v>0.9</v>
       </c>
       <c r="L77" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="N77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>2</v>
@@ -4572,13 +4735,19 @@
         <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
+      <c r="L78" t="s">
+        <v>216</v>
+      </c>
       <c r="N78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -4615,13 +4784,19 @@
         <f t="shared" si="11"/>
         <v>1.8</v>
       </c>
+      <c r="L79" t="s">
+        <v>207</v>
+      </c>
       <c r="N79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -4658,13 +4833,19 @@
         <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
+      <c r="L80" t="s">
+        <v>208</v>
+      </c>
       <c r="N80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -4702,15 +4883,18 @@
         <v>0.9</v>
       </c>
       <c r="L81" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="N81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="B82">
         <v>2</v>
@@ -4748,15 +4932,18 @@
         <v>0.9</v>
       </c>
       <c r="L82" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="N82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -4794,15 +4981,18 @@
         <v>0.9</v>
       </c>
       <c r="L83" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="N83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B84">
         <v>2</v>
@@ -4839,13 +5029,19 @@
         <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
-      <c r="N84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L84" t="s">
+        <v>158</v>
+      </c>
+      <c r="N84" s="10">
+        <v>1</v>
+      </c>
+      <c r="O84" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>221</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -4882,13 +5078,19 @@
         <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
+      <c r="L85" t="s">
+        <v>222</v>
+      </c>
       <c r="N85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B86">
         <v>2</v>
@@ -4925,13 +5127,16 @@
         <f t="shared" si="11"/>
         <v>0.9</v>
       </c>
-      <c r="N86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9">
+        <v>1</v>
+      </c>
+      <c r="O86" s="9"/>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B87">
         <v>2</v>
@@ -4970,9 +5175,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -5009,13 +5214,19 @@
         <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
+      <c r="L88" t="s">
+        <v>217</v>
+      </c>
       <c r="N88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -5054,9 +5265,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B90">
         <v>2</v>
@@ -5095,9 +5306,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B91">
         <v>2</v>
@@ -5134,13 +5345,19 @@
         <f t="shared" si="11"/>
         <v>1.8</v>
       </c>
+      <c r="L91" t="s">
+        <v>220</v>
+      </c>
       <c r="N91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -5179,9 +5396,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B93">
         <v>2</v>
@@ -5220,9 +5437,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15">
       <c r="A94" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -5261,7 +5478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15">
       <c r="C95">
         <f t="shared" si="7"/>
         <v>0</v>
@@ -5287,9 +5504,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15">
       <c r="A96" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C96">
         <f>SUM(G97:G111)</f>
@@ -5316,9 +5533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15">
       <c r="A97" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -5356,15 +5573,18 @@
         <v>1</v>
       </c>
       <c r="L97" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="N97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -5402,15 +5622,18 @@
         <v>1.6</v>
       </c>
       <c r="L98" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="N98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -5448,15 +5671,18 @@
         <v>1.6</v>
       </c>
       <c r="L99" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="N99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -5494,15 +5720,18 @@
         <v>0.8</v>
       </c>
       <c r="L100" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="N100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -5540,15 +5769,18 @@
         <v>1.6</v>
       </c>
       <c r="L101" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="N101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>209</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -5586,15 +5818,18 @@
         <v>1.6</v>
       </c>
       <c r="L102" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="N102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -5632,15 +5867,18 @@
         <v>1.6</v>
       </c>
       <c r="L103" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="N103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -5678,15 +5916,18 @@
         <v>1.6</v>
       </c>
       <c r="L104" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="N104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -5724,15 +5965,18 @@
         <v>1</v>
       </c>
       <c r="L105" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="N105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -5770,15 +6014,18 @@
         <v>0.5</v>
       </c>
       <c r="L106" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="N106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -5816,15 +6063,18 @@
         <v>1.6</v>
       </c>
       <c r="L107" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="N107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -5862,15 +6112,18 @@
         <v>1.6</v>
       </c>
       <c r="L108" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="N108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -5908,12 +6161,18 @@
         <v>0.9</v>
       </c>
       <c r="L109" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="N109">
+        <v>1</v>
+      </c>
+      <c r="O109" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -5951,15 +6210,18 @@
         <v>0.8</v>
       </c>
       <c r="L110" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="N110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>203</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -5997,15 +6259,18 @@
         <v>1.6</v>
       </c>
       <c r="L111" t="s">
+        <v>189</v>
+      </c>
+      <c r="N111">
+        <v>1</v>
+      </c>
+      <c r="O111" t="s">
         <v>202</v>
       </c>
-      <c r="N111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
-        <v>116</v>
+        <v>204</v>
       </c>
       <c r="B112">
         <v>2</v>
@@ -6043,15 +6308,18 @@
         <v>1.6</v>
       </c>
       <c r="L112" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="N112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B113">
         <v>2</v>
@@ -6077,15 +6345,18 @@
         <v>1.6</v>
       </c>
       <c r="L113" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="N113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="B114">
         <v>2</v>
@@ -6111,15 +6382,18 @@
         <v>1.6</v>
       </c>
       <c r="L114" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="N114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
-        <v>118</v>
+        <v>212</v>
       </c>
       <c r="B115">
         <v>2</v>
@@ -6131,29 +6405,32 @@
         <v>3</v>
       </c>
       <c r="E115">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F115">
         <v>80</v>
       </c>
       <c r="G115">
         <f t="shared" si="17"/>
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="K115">
         <f t="shared" si="11"/>
-        <v>1.6</v>
+        <v>3.2</v>
       </c>
       <c r="L115" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="N115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
-        <v>119</v>
+        <v>213</v>
       </c>
       <c r="B116">
         <v>2</v>
@@ -6165,29 +6442,32 @@
         <v>3</v>
       </c>
       <c r="E116">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F116">
         <v>20</v>
       </c>
       <c r="G116">
         <f t="shared" si="17"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="K116">
         <f t="shared" si="11"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="L116" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="N116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B117">
         <v>2</v>
@@ -6213,15 +6493,18 @@
         <v>1.2</v>
       </c>
       <c r="L117" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="N117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="B118">
         <v>2</v>
@@ -6247,15 +6530,18 @@
         <v>1.6</v>
       </c>
       <c r="L118" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="N118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B119">
         <v>2</v>
@@ -6282,9 +6568,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B120">
         <v>2</v>
@@ -6322,15 +6608,18 @@
         <v>0.8</v>
       </c>
       <c r="L120" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="N120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B121">
         <v>2</v>
@@ -6368,15 +6657,18 @@
         <v>1.6</v>
       </c>
       <c r="L121" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="N121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15">
       <c r="A122" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B122">
         <v>2</v>
@@ -6414,15 +6706,18 @@
         <v>1.6</v>
       </c>
       <c r="L122" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="N122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B123">
         <v>2</v>
@@ -6459,13 +6754,19 @@
         <f t="shared" si="21"/>
         <v>0.8</v>
       </c>
+      <c r="L123" t="s">
+        <v>215</v>
+      </c>
       <c r="N123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B124">
         <v>2</v>
@@ -6504,9 +6805,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B125">
         <v>2</v>
@@ -6545,9 +6846,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15">
       <c r="A126" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B126">
         <v>2</v>
@@ -6586,7 +6887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15">
       <c r="C127">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -6612,9 +6913,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15">
       <c r="A128" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C128">
         <f t="shared" si="26"/>
@@ -6641,9 +6942,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -6681,15 +6982,18 @@
         <v>1</v>
       </c>
       <c r="L129" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O129" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -6727,15 +7031,18 @@
         <v>1.6</v>
       </c>
       <c r="L130" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="N130">
         <v>1</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O130" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -6773,15 +7080,18 @@
         <v>1.8</v>
       </c>
       <c r="L131" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O131" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -6819,15 +7129,18 @@
         <v>1.8</v>
       </c>
       <c r="L132" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O132" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -6865,15 +7178,18 @@
         <v>1.8</v>
       </c>
       <c r="L133" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O133" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -6911,15 +7227,18 @@
         <v>1.8</v>
       </c>
       <c r="L134" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O134" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -6957,15 +7276,18 @@
         <v>1.8</v>
       </c>
       <c r="L135" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O135" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -7004,9 +7326,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -7045,9 +7367,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15">
       <c r="A138" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -7085,9 +7407,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -7125,15 +7447,18 @@
         <v>1.8</v>
       </c>
       <c r="L139" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N139">
         <v>1</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O139" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -7171,15 +7496,18 @@
         <v>1.8</v>
       </c>
       <c r="L140" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="N140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O140" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15">
       <c r="A141" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -7218,10 +7546,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15">
       <c r="N142">
         <f>SUM(N1:N141)</f>
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated more save the date stuff
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="228">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -700,6 +700,9 @@
   </si>
   <si>
     <t>3113 Gillespie St., Houston, TX 77020</t>
+  </si>
+  <si>
+    <t>Logan has to deliver</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1331,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1339,8 +1342,8 @@
   <dimension ref="A1:S142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O42" sqref="L42:O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1988,9 +1991,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="N16">
-        <v>1</v>
-      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8">
+        <v>1</v>
+      </c>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
@@ -2031,9 +2037,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N17">
-        <v>1</v>
-      </c>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8">
+        <v>1</v>
+      </c>
+      <c r="O17" s="8"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
@@ -2166,9 +2175,12 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="N20">
-        <v>1</v>
-      </c>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8">
+        <v>1</v>
+      </c>
+      <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
@@ -2209,9 +2221,12 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8">
+        <v>1</v>
+      </c>
+      <c r="O21" s="8"/>
     </row>
     <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
@@ -2347,9 +2362,12 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8">
+        <v>1</v>
+      </c>
+      <c r="O24" s="8"/>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">
@@ -3193,12 +3211,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M42" t="s">
+      <c r="L42" s="8"/>
+      <c r="M42" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="N42">
-        <v>1</v>
-      </c>
+      <c r="N42" s="8">
+        <v>1</v>
+      </c>
+      <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15">
       <c r="A43" t="s">
@@ -3715,7 +3735,9 @@
       <c r="N55" s="8">
         <v>1</v>
       </c>
-      <c r="O55" s="8"/>
+      <c r="O55" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="56" spans="1:15">
       <c r="A56" t="s">
@@ -3813,7 +3835,9 @@
       <c r="N57" s="8">
         <v>1</v>
       </c>
-      <c r="O57" s="8"/>
+      <c r="O57" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="58" spans="1:15">
       <c r="A58" t="s">
@@ -4112,7 +4136,9 @@
       <c r="N64" s="8">
         <v>1</v>
       </c>
-      <c r="O64" s="8"/>
+      <c r="O64" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="65" spans="1:15">
       <c r="A65" t="s">
@@ -4211,7 +4237,9 @@
       <c r="N66" s="8">
         <v>1</v>
       </c>
-      <c r="O66" s="8"/>
+      <c r="O66" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="67" spans="1:15">
       <c r="A67" t="s">
@@ -4259,7 +4287,9 @@
       <c r="N67" s="8">
         <v>1</v>
       </c>
-      <c r="O67" s="8"/>
+      <c r="O67" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="68" spans="1:15">
       <c r="A68" t="s">
@@ -4429,7 +4459,9 @@
       <c r="N71" s="8">
         <v>1</v>
       </c>
-      <c r="O71" s="8"/>
+      <c r="O71" s="8" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="72" spans="1:15">
       <c r="A72" t="s">

</xml_diff>

<commit_message>
Updated for things sent
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\logan\Documents\GitHub\Farrell_Garrett_Wedding\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="247">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -762,13 +757,16 @@
   </si>
   <si>
     <t>P.O. Box 296, Milton, IN 47357</t>
+  </si>
+  <si>
+    <t>Need address after she moves</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -786,6 +784,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -847,7 +852,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -858,10 +863,11 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1391,36 +1397,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35.85546875" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" customWidth="1"/>
     <col min="8" max="11" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="35.5703125" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="15" max="15" width="11" customWidth="1"/>
     <col min="16" max="16" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" s="7">
         <v>4</v>
       </c>
@@ -1447,17 +1453,17 @@
         <f>SUMIF(D6:D224,"&gt;3",E6:E224)</f>
         <v>130</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="6">
         <v>3</v>
       </c>
@@ -1476,11 +1482,11 @@
       <c r="G2" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1507,9 +1513,9 @@
         <f>SUM(J:J)</f>
         <v>85.499999999999915</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
       <c r="R3" t="s">
         <v>38</v>
       </c>
@@ -1517,7 +1523,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1557,11 +1563,11 @@
       <c r="M4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1570,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1619,7 +1625,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1674,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1717,7 +1723,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1766,7 +1772,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1854,6 +1860,9 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
+      <c r="L11" s="12" t="s">
+        <v>246</v>
+      </c>
       <c r="N11">
         <v>1</v>
       </c>
@@ -1861,7 +1870,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="B12" s="1"/>
       <c r="C12">
         <f t="shared" ref="C12:C62" si="5">IF(D12=4, 1,0)</f>
@@ -1888,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1917,7 +1926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1966,7 +1975,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
@@ -2015,7 +2024,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2054,7 +2063,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="10" t="s">
         <v>244</v>
       </c>
       <c r="M16" s="9"/>
@@ -2065,7 +2074,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
@@ -2111,7 +2120,7 @@
       </c>
       <c r="O17" s="9"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="2" t="s">
         <v>237</v>
       </c>
@@ -2259,7 +2268,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15">
       <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
@@ -2298,14 +2307,18 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8">
-        <v>1</v>
-      </c>
-      <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L21" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9">
+        <v>1</v>
+      </c>
+      <c r="O21" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -2354,7 +2367,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
@@ -2403,7 +2416,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="A24" s="2" t="s">
         <v>19</v>
       </c>
@@ -2451,7 +2464,7 @@
       </c>
       <c r="O24" s="8"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">
         <v>20</v>
       </c>
@@ -2500,7 +2513,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -2549,7 +2562,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -2598,7 +2611,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15">
       <c r="A28" s="2" t="s">
         <v>23</v>
       </c>
@@ -2647,7 +2660,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
@@ -2696,7 +2709,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15">
       <c r="A30" s="2" t="s">
         <v>25</v>
       </c>
@@ -2745,7 +2758,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15">
       <c r="A31" s="2" t="s">
         <v>26</v>
       </c>
@@ -2794,7 +2807,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15">
       <c r="A32" s="2" t="s">
         <v>27</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" s="2" t="s">
         <v>28</v>
       </c>
@@ -2892,7 +2905,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" s="2" t="s">
         <v>29</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" s="2" t="s">
         <v>43</v>
       </c>
@@ -2990,7 +3003,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
@@ -3039,7 +3052,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" s="2" t="s">
         <v>45</v>
       </c>
@@ -3088,7 +3101,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" s="2" t="s">
         <v>46</v>
       </c>
@@ -3137,7 +3150,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -3186,7 +3199,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" s="2" t="s">
         <v>48</v>
       </c>
@@ -3235,7 +3248,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -3284,7 +3297,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -3332,7 +3345,7 @@
       </c>
       <c r="O42" s="8"/>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>138</v>
       </c>
@@ -3381,7 +3394,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" s="2"/>
       <c r="C44">
         <f t="shared" si="5"/>
@@ -3408,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="B45" s="1"/>
       <c r="C45">
         <f t="shared" si="5"/>
@@ -3435,7 +3448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" s="1" t="s">
         <v>30</v>
       </c>
@@ -3463,11 +3476,8 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -3515,8 +3525,11 @@
       <c r="N47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O47" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -3564,8 +3577,11 @@
       <c r="N48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O48" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -3613,8 +3629,11 @@
       <c r="N49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O49" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50" t="s">
         <v>34</v>
       </c>
@@ -3662,8 +3681,11 @@
       <c r="N50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O50" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51" t="s">
         <v>35</v>
       </c>
@@ -3711,8 +3733,11 @@
       <c r="N51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O51" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52" t="s">
         <v>36</v>
       </c>
@@ -3751,14 +3776,16 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="M52" t="s">
+      <c r="L52" s="8"/>
+      <c r="M52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="N52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N52" s="8">
+        <v>1</v>
+      </c>
+      <c r="O52" s="8"/>
+    </row>
+    <row r="53" spans="1:15">
       <c r="C53">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3784,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15">
       <c r="A54" s="1" t="s">
         <v>57</v>
       </c>
@@ -3813,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -3863,7 +3890,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15">
       <c r="A56" t="s">
         <v>59</v>
       </c>
@@ -3913,7 +3940,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -3963,7 +3990,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15">
       <c r="A58" t="s">
         <v>99</v>
       </c>
@@ -4012,7 +4039,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -4061,7 +4088,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -4110,7 +4137,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -4159,7 +4186,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15">
       <c r="C62">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -4185,7 +4212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15">
       <c r="A63" s="1" t="s">
         <v>55</v>
       </c>
@@ -4214,7 +4241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -4264,7 +4291,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -4313,7 +4340,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -4365,7 +4392,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -4415,7 +4442,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15">
       <c r="A68" t="s">
         <v>213</v>
       </c>
@@ -4464,7 +4491,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15">
       <c r="A69" t="s">
         <v>240</v>
       </c>
@@ -4488,7 +4515,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -4537,7 +4564,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -4587,7 +4614,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -4636,7 +4663,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -4685,7 +4712,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -4734,7 +4761,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -4783,7 +4810,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -4832,7 +4859,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -4881,7 +4908,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -4930,7 +4957,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15">
       <c r="A79" t="s">
         <v>212</v>
       </c>
@@ -4979,7 +5006,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -5028,7 +5055,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -5077,7 +5104,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -5126,7 +5153,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15">
       <c r="A83" t="s">
         <v>77</v>
       </c>
@@ -5175,7 +5202,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15">
       <c r="A84" t="s">
         <v>215</v>
       </c>
@@ -5224,7 +5251,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15">
       <c r="A85" t="s">
         <v>161</v>
       </c>
@@ -5274,7 +5301,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -5315,7 +5342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15">
       <c r="A87" t="s">
         <v>81</v>
       </c>
@@ -5364,7 +5391,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15">
       <c r="A88" t="s">
         <v>160</v>
       </c>
@@ -5405,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15">
       <c r="A89" t="s">
         <v>82</v>
       </c>
@@ -5446,7 +5473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -5495,7 +5522,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -5536,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -5577,7 +5604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -5618,7 +5645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15">
       <c r="C94">
         <f t="shared" si="12"/>
         <v>0</v>
@@ -5644,7 +5671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15">
       <c r="A95" s="1" t="s">
         <v>95</v>
       </c>
@@ -5673,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15">
       <c r="A96" s="2" t="s">
         <v>102</v>
       </c>
@@ -5722,7 +5749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -5771,7 +5798,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15">
       <c r="A98" t="s">
         <v>180</v>
       </c>
@@ -5820,7 +5847,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -5869,7 +5896,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -5918,7 +5945,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15">
       <c r="A101" t="s">
         <v>203</v>
       </c>
@@ -5967,7 +5994,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -6016,7 +6043,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15">
       <c r="A103" t="s">
         <v>204</v>
       </c>
@@ -6065,7 +6092,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15">
       <c r="A104" t="s">
         <v>164</v>
       </c>
@@ -6114,7 +6141,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15">
       <c r="A105" t="s">
         <v>181</v>
       </c>
@@ -6163,7 +6190,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15">
       <c r="A106" t="s">
         <v>100</v>
       </c>
@@ -6212,7 +6239,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15">
       <c r="A107" t="s">
         <v>205</v>
       </c>
@@ -6261,7 +6288,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15">
       <c r="A108" t="s">
         <v>193</v>
       </c>
@@ -6310,7 +6337,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15">
       <c r="A109" t="s">
         <v>101</v>
       </c>
@@ -6359,7 +6386,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15">
       <c r="A110" t="s">
         <v>197</v>
       </c>
@@ -6408,7 +6435,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15">
       <c r="A111" t="s">
         <v>198</v>
       </c>
@@ -6457,7 +6484,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -6494,7 +6521,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15">
       <c r="A113" t="s">
         <v>157</v>
       </c>
@@ -6531,7 +6558,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15">
       <c r="A114" t="s">
         <v>206</v>
       </c>
@@ -6568,7 +6595,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15">
       <c r="A115" t="s">
         <v>207</v>
       </c>
@@ -6605,7 +6632,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15">
       <c r="A116" t="s">
         <v>109</v>
       </c>
@@ -6642,7 +6669,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15">
       <c r="A117" t="s">
         <v>162</v>
       </c>
@@ -6679,7 +6706,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15">
       <c r="A118" t="s">
         <v>110</v>
       </c>
@@ -6708,7 +6735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15">
       <c r="A119" t="s">
         <v>112</v>
       </c>
@@ -6757,7 +6784,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15">
       <c r="A120" t="s">
         <v>104</v>
       </c>
@@ -6806,7 +6833,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15">
       <c r="A121" t="s">
         <v>105</v>
       </c>
@@ -6855,7 +6882,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15">
       <c r="A122" t="s">
         <v>111</v>
       </c>
@@ -6904,7 +6931,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15">
       <c r="A123" t="s">
         <v>106</v>
       </c>
@@ -6945,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15">
       <c r="A124" t="s">
         <v>113</v>
       </c>
@@ -6986,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15">
       <c r="A125" t="s">
         <v>107</v>
       </c>
@@ -7027,7 +7054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15">
       <c r="C126">
         <f t="shared" si="26"/>
         <v>0</v>
@@ -7053,7 +7080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15">
       <c r="A127" s="1" t="s">
         <v>114</v>
       </c>
@@ -7082,7 +7109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -7131,7 +7158,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15">
       <c r="A129" t="s">
         <v>116</v>
       </c>
@@ -7180,7 +7207,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15">
       <c r="A130" t="s">
         <v>117</v>
       </c>
@@ -7229,7 +7256,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15">
       <c r="A131" t="s">
         <v>118</v>
       </c>
@@ -7278,7 +7305,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15">
       <c r="A132" t="s">
         <v>119</v>
       </c>
@@ -7327,7 +7354,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15">
       <c r="A133" t="s">
         <v>120</v>
       </c>
@@ -7376,7 +7403,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15">
       <c r="A134" t="s">
         <v>121</v>
       </c>
@@ -7425,7 +7452,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15">
       <c r="A135" t="s">
         <v>163</v>
       </c>
@@ -7465,7 +7492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15">
       <c r="A136" t="s">
         <v>122</v>
       </c>
@@ -7514,7 +7541,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15">
       <c r="A137" t="s">
         <v>123</v>
       </c>
@@ -7563,10 +7590,10 @@
         <v>218</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15">
       <c r="N138">
         <f>SUM(N1:N137)</f>
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Mr. Klumpe's address
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="249">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -760,6 +760,12 @@
   </si>
   <si>
     <t>Need address after she moves</t>
+  </si>
+  <si>
+    <t>5509 N 200 E, Attica, IN 47918</t>
+  </si>
+  <si>
+    <t>Hand deliver</t>
   </si>
 </sst>
 </file>
@@ -864,10 +870,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1397,7 +1403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1408,8 +1414,8 @@
   <dimension ref="A1:S138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M46" sqref="M46"/>
+      <pane ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O53" sqref="O53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1453,13 +1459,13 @@
         <f>SUMIF(D6:D224,"&gt;3",E6:E224)</f>
         <v>130</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="O1" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P1" s="12" t="s">
         <v>170</v>
       </c>
     </row>
@@ -1482,9 +1488,9 @@
       <c r="G2" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="4">
@@ -1513,9 +1519,9 @@
         <f>SUM(J:J)</f>
         <v>85.499999999999915</v>
       </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
       <c r="R3" t="s">
         <v>38</v>
       </c>
@@ -1563,9 +1569,9 @@
       <c r="M4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="1" t="s">
@@ -1860,7 +1866,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L11" s="12" t="s">
+      <c r="L11" s="11" t="s">
         <v>246</v>
       </c>
       <c r="N11">
@@ -3776,14 +3782,18 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L52" s="8"/>
-      <c r="M52" s="8" t="s">
+      <c r="L52" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="M52" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="N52" s="8">
-        <v>1</v>
-      </c>
-      <c r="O52" s="8"/>
+      <c r="N52" s="9">
+        <v>1</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="53" spans="1:15">
       <c r="C53">

</xml_diff>

<commit_message>
Updated Save the Date info
</commit_message>
<xml_diff>
--- a/Guest_List_Initial.xlsx
+++ b/Guest_List_Initial.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="249">
   <si>
     <t xml:space="preserve">Priority </t>
   </si>
@@ -1403,7 +1403,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1414,8 +1414,8 @@
   <dimension ref="A1:S138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O53" sqref="O53"/>
+      <pane ySplit="4" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P128" sqref="P128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2461,14 +2461,16 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8">
-        <v>1</v>
-      </c>
-      <c r="O24" s="8"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9">
+        <v>1</v>
+      </c>
+      <c r="O24" s="9" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" s="2" t="s">

</xml_diff>